<commit_message>
leetcode potd palindrome substrings
</commit_message>
<xml_diff>
--- a/Daily Log.xlsx
+++ b/Daily Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Utkarsh\Daily Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665B2574-2FDD-468B-9462-F330AFD8CB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB7730A-BC5A-4198-B642-260EF9AC6C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4387,12 +4387,61 @@
         </r>
       </text>
     </comment>
+    <comment ref="I94" authorId="0" shapeId="0" xr:uid="{C8D5238B-E3D7-48B7-9124-68ADEB2C6B62}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+class Solution {
+public:
+    int countSubstrings(string s) {
+        int n=s.length();
+        bool dp[n][n];
+        int count=0;
+        for(int gap=0;gap&lt;n;gap++){
+            // here i points to starting point of a substring
+            // and j points to end point of a substirng
+            for(int i =0, j=gap; j&lt;n;i++, j++){
+                if(gap==0)//ie if length of substring is 1 then it will always be palindrome
+                {
+                    dp[i][j]=true;
+                }else if(gap==1){
+                    dp[i][j]=s[i]==s[j];
+                }else{
+                    if(s[i]==s[j]){
+                        dp[i][j]=dp[i+1][j-1];
+                    }else dp[i][j]=false;
+                }
+                if(dp[i][j])count++;
+            }
+        }
+        return count;
+    }
+};</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="206">
   <si>
     <t>what you did today</t>
   </si>
@@ -5662,6 +5711,16 @@
   <si>
     <t>create a map with key=string and value=vector now we iterate the given vector of string (strs) for every string we sort that string and store it in map as key and push_back the original string (before sort) in value vector of map.
 If the key does not already exist in map we create a vetorand push the string and then store it to map</t>
+  </si>
+  <si>
+    <t>Palindromic Substrings</t>
+  </si>
+  <si>
+    <t>we create a dp[n][n] 
+1) start a loop of gap=0 to n where gap indicate length of substring 
+2) start innner loop with i=0 and j=gap here I to j gives a substring of length gap+1;
+3) now we check if gap ==0 ie length of string is 1 then it is always palindrome also if gap==1 ie. length =2 then if both are equal then it is palindrome we check it and mark that d[i][j]=true
+4)if gap is grater than 1 than we check if last two(s[i]&amp;s[j]) of substring are equal or not and then for subtring in between we check it in dp(ie dp[i+1][j-1]) if that is true than this one is also palindrome</t>
   </si>
 </sst>
 </file>
@@ -6116,8 +6175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:I179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H96" sqref="H96"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H97" sqref="H97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8214,9 +8273,28 @@
         <v>203</v>
       </c>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B94" s="6"/>
-      <c r="H94" s="3"/>
+    <row r="94" spans="2:9" ht="144" x14ac:dyDescent="0.3">
+      <c r="B94" s="6">
+        <v>92</v>
+      </c>
+      <c r="C94" s="2">
+        <v>45332</v>
+      </c>
+      <c r="D94" t="s">
+        <v>85</v>
+      </c>
+      <c r="E94" t="s">
+        <v>46</v>
+      </c>
+      <c r="F94" t="s">
+        <v>15</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B95" s="7"/>
@@ -8649,12 +8727,13 @@
     <hyperlink ref="G91" r:id="rId86" display="https://leetcode.com/problems/daily-temperatures/" xr:uid="{88D67DE6-DAD0-4CB2-87EA-20F6D9D92E5D}"/>
     <hyperlink ref="G92" r:id="rId87" display="https://leetcode.com/problems/unique-paths/" xr:uid="{75EFC9D3-2184-4D14-A773-203CAF78B1FE}"/>
     <hyperlink ref="G93" r:id="rId88" display="https://leetcode.com/problems/group-anagrams/" xr:uid="{88ADF45E-CABB-4BE8-8ABF-879E4531F0BE}"/>
+    <hyperlink ref="G94" r:id="rId89" display="https://leetcode.com/problems/palindromic-substrings/" xr:uid="{50118B62-0520-4187-9C28-32DDF5137AA3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId89"/>
-  <legacyDrawing r:id="rId90"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId90"/>
+  <legacyDrawing r:id="rId91"/>
   <tableParts count="1">
-    <tablePart r:id="rId91"/>
+    <tablePart r:id="rId92"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
potd Least Number of Unique Integers after K Removals
</commit_message>
<xml_diff>
--- a/Daily Log.xlsx
+++ b/Daily Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Utkarsh\Daily Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB7730A-BC5A-4198-B642-260EF9AC6C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCD53EF-1A20-41A0-BDE9-B04B5A813E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4436,12 +4436,57 @@
         </r>
       </text>
     </comment>
+    <comment ref="I95" authorId="0" shapeId="0" xr:uid="{F9E98A77-F6FC-4EC4-A62A-3C007E059C56}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+class Solution {
+public:
+    int findLeastNumOfUniqueInts(vector&lt;int&gt;&amp; arr, int k) {
+        unordered_map&lt;int, int&gt; mp;
+        for (auto it : arr) {
+            mp[it]++;
+        }
+        vector&lt;int&gt; v;
+        for (auto it : mp) {
+            v.push_back(it.second);
+        }
+        sort(v.begin(), v.end());
+        int cnt =v.size();
+        for (auto it: v){
+            if((k-it)&gt;=0){
+                k=k-it;
+                cnt--;
+            }else break;
+        }
+        return cnt;
+    }
+};</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="208">
   <si>
     <t>what you did today</t>
   </si>
@@ -5721,6 +5766,19 @@
 2) start innner loop with i=0 and j=gap here I to j gives a substring of length gap+1;
 3) now we check if gap ==0 ie length of string is 1 then it is always palindrome also if gap==1 ie. length =2 then if both are equal then it is palindrome we check it and mark that d[i][j]=true
 4)if gap is grater than 1 than we check if last two(s[i]&amp;s[j]) of substring are equal or not and then for subtring in between we check it in dp(ie dp[i+1][j-1]) if that is true than this one is also palindrome</t>
+  </si>
+  <si>
+    <t>Least Number of Unique Integers after K Removals</t>
+  </si>
+  <si>
+    <t>Create a map and store the frequency of each element of arr
+Now for every key-value pair of map store values in a vector v
+sort the vector v
+create a cnt=v.size();
+iterate the vector and check k-v[i]
+    if it is &gt;= 0 than k=k-v[i] and cnt--.
+    else break.
+return cnt;</t>
   </si>
 </sst>
 </file>
@@ -6175,8 +6233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:I179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H97" sqref="H97"/>
+    <sheetView tabSelected="1" topLeftCell="F94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H98" sqref="H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8296,9 +8354,28 @@
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B95" s="7"/>
-      <c r="H95" s="3"/>
+    <row r="95" spans="2:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B95" s="7">
+        <v>93</v>
+      </c>
+      <c r="C95" s="2">
+        <v>45338</v>
+      </c>
+      <c r="D95" t="s">
+        <v>85</v>
+      </c>
+      <c r="E95" t="s">
+        <v>46</v>
+      </c>
+      <c r="F95" t="s">
+        <v>15</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H95" s="3" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B96" s="6"/>
@@ -8728,12 +8805,13 @@
     <hyperlink ref="G92" r:id="rId87" display="https://leetcode.com/problems/unique-paths/" xr:uid="{75EFC9D3-2184-4D14-A773-203CAF78B1FE}"/>
     <hyperlink ref="G93" r:id="rId88" display="https://leetcode.com/problems/group-anagrams/" xr:uid="{88ADF45E-CABB-4BE8-8ABF-879E4531F0BE}"/>
     <hyperlink ref="G94" r:id="rId89" display="https://leetcode.com/problems/palindromic-substrings/" xr:uid="{50118B62-0520-4187-9C28-32DDF5137AA3}"/>
+    <hyperlink ref="G95" r:id="rId90" xr:uid="{43BA1C6C-4023-4FE5-BE8F-7D9047EF92D5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId90"/>
-  <legacyDrawing r:id="rId91"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId91"/>
+  <legacyDrawing r:id="rId92"/>
   <tableParts count="1">
-    <tablePart r:id="rId92"/>
+    <tablePart r:id="rId93"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>